<commit_message>
update csv/model/ CIMS_DCC, CIMS_FIC, CIMS_DIC, CIMS_market share limits
</commit_message>
<xml_diff>
--- a/csv/model/CIMS_DCC/formula_CIMS_DCC_AB.xlsx
+++ b/csv/model/CIMS_DCC/formula_CIMS_DCC_AB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\xCIMS\cims-models\csv\model\CIMS_DCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9028E13-37E2-4A2D-992B-5960D8CA9334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{33F27A48-A225-40C8-A425-FA062751F472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{31F2F843-8D8D-461A-9C26-6FCD32A798BE}"/>
+    <workbookView xWindow="41850" yWindow="4965" windowWidth="17280" windowHeight="8880" xr2:uid="{16DEA2D2-60EE-4D25-91F0-F5ECF3A90052}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -652,21 +652,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFA165CC-8775-4506-B9ED-33EA28631077}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2022D3-7CF9-4390-A02B-B9B96D39752A}">
   <dimension ref="A1:X88"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:X88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -740,7 +740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -799,7 +799,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -858,7 +858,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -917,7 +917,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -976,7 +976,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>6840</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>17.009699999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>3.62</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>15.8757</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>66</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>66</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>66</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>66</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>66</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>66</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -3900,7 +3900,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>66</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>66</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>72</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>72</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -5039,7 +5039,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -5246,7 +5246,7 @@
         <v>54000000</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -5315,7 +5315,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -5341,7 +5341,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>78</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>78</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>80</v>
       </c>
@@ -5712,7 +5712,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>80</v>
       </c>
@@ -5781,7 +5781,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>80</v>
       </c>
@@ -5850,7 +5850,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>80</v>
       </c>

</xml_diff>